<commit_message>
Adding new updated data files.
</commit_message>
<xml_diff>
--- a/data/fitness_development/fly_part2.xlsx
+++ b/data/fitness_development/fly_part2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_13/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDFC7D96-F01D-DA4A-B785-D050D82E65BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED272A5-4B2B-254D-B2EA-C81B42521305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BB242E00-5CB3-A84F-BA7A-96A75344F1EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB267A-8CE1-0F4E-97AE-D44F1974EE08}">
-  <dimension ref="A1:E273"/>
+  <dimension ref="A1:E409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="176" workbookViewId="0">
-      <selection activeCell="F270" sqref="F270"/>
+    <sheetView tabSelected="1" topLeftCell="A387" zoomScale="163" workbookViewId="0">
+      <selection activeCell="E409" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5080,6 +5080,2318 @@
         <v>0</v>
       </c>
     </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>1</v>
+      </c>
+      <c r="B274" t="s">
+        <v>5</v>
+      </c>
+      <c r="C274">
+        <v>236</v>
+      </c>
+      <c r="D274">
+        <v>0</v>
+      </c>
+      <c r="E274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>1</v>
+      </c>
+      <c r="B275" t="s">
+        <v>6</v>
+      </c>
+      <c r="C275">
+        <v>236</v>
+      </c>
+      <c r="D275">
+        <v>0</v>
+      </c>
+      <c r="E275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>2</v>
+      </c>
+      <c r="B276" t="s">
+        <v>5</v>
+      </c>
+      <c r="C276">
+        <v>236</v>
+      </c>
+      <c r="D276">
+        <v>0</v>
+      </c>
+      <c r="E276">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>2</v>
+      </c>
+      <c r="B277" t="s">
+        <v>6</v>
+      </c>
+      <c r="C277">
+        <v>236</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+      <c r="E277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>3</v>
+      </c>
+      <c r="B278" t="s">
+        <v>5</v>
+      </c>
+      <c r="C278">
+        <v>236</v>
+      </c>
+      <c r="D278">
+        <v>0</v>
+      </c>
+      <c r="E278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>3</v>
+      </c>
+      <c r="B279" t="s">
+        <v>6</v>
+      </c>
+      <c r="C279">
+        <v>236</v>
+      </c>
+      <c r="D279">
+        <v>3</v>
+      </c>
+      <c r="E279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>4</v>
+      </c>
+      <c r="B280" t="s">
+        <v>5</v>
+      </c>
+      <c r="C280">
+        <v>236</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+      <c r="E280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>4</v>
+      </c>
+      <c r="B281" t="s">
+        <v>6</v>
+      </c>
+      <c r="C281">
+        <v>236</v>
+      </c>
+      <c r="D281">
+        <v>0</v>
+      </c>
+      <c r="E281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>5</v>
+      </c>
+      <c r="B282" t="s">
+        <v>5</v>
+      </c>
+      <c r="C282">
+        <v>236</v>
+      </c>
+      <c r="D282">
+        <v>1</v>
+      </c>
+      <c r="E282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>5</v>
+      </c>
+      <c r="B283" t="s">
+        <v>6</v>
+      </c>
+      <c r="C283">
+        <v>236</v>
+      </c>
+      <c r="D283">
+        <v>0</v>
+      </c>
+      <c r="E283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>6</v>
+      </c>
+      <c r="B284" t="s">
+        <v>5</v>
+      </c>
+      <c r="C284">
+        <v>236</v>
+      </c>
+      <c r="D284">
+        <v>1</v>
+      </c>
+      <c r="E284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>6</v>
+      </c>
+      <c r="B285" t="s">
+        <v>6</v>
+      </c>
+      <c r="C285">
+        <v>236</v>
+      </c>
+      <c r="D285">
+        <v>0</v>
+      </c>
+      <c r="E285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>7</v>
+      </c>
+      <c r="B286" t="s">
+        <v>5</v>
+      </c>
+      <c r="C286">
+        <v>236</v>
+      </c>
+      <c r="D286">
+        <v>0</v>
+      </c>
+      <c r="E286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>7</v>
+      </c>
+      <c r="B287" t="s">
+        <v>6</v>
+      </c>
+      <c r="C287">
+        <v>236</v>
+      </c>
+      <c r="D287">
+        <v>1</v>
+      </c>
+      <c r="E287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>8</v>
+      </c>
+      <c r="B288" t="s">
+        <v>5</v>
+      </c>
+      <c r="C288">
+        <v>236</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+      <c r="E288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>8</v>
+      </c>
+      <c r="B289" t="s">
+        <v>6</v>
+      </c>
+      <c r="C289">
+        <v>236</v>
+      </c>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>9</v>
+      </c>
+      <c r="B290" t="s">
+        <v>5</v>
+      </c>
+      <c r="C290">
+        <v>236</v>
+      </c>
+      <c r="D290">
+        <v>2</v>
+      </c>
+      <c r="E290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>9</v>
+      </c>
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291">
+        <v>236</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>10</v>
+      </c>
+      <c r="B292" t="s">
+        <v>5</v>
+      </c>
+      <c r="C292">
+        <v>236</v>
+      </c>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>10</v>
+      </c>
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293">
+        <v>236</v>
+      </c>
+      <c r="D293">
+        <v>1</v>
+      </c>
+      <c r="E293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>11</v>
+      </c>
+      <c r="B294" t="s">
+        <v>5</v>
+      </c>
+      <c r="C294">
+        <v>236</v>
+      </c>
+      <c r="D294">
+        <v>1</v>
+      </c>
+      <c r="E294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>11</v>
+      </c>
+      <c r="B295" t="s">
+        <v>6</v>
+      </c>
+      <c r="C295">
+        <v>236</v>
+      </c>
+      <c r="D295">
+        <v>1</v>
+      </c>
+      <c r="E295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>12</v>
+      </c>
+      <c r="B296" t="s">
+        <v>5</v>
+      </c>
+      <c r="C296">
+        <v>236</v>
+      </c>
+      <c r="D296">
+        <v>2</v>
+      </c>
+      <c r="E296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>12</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297">
+        <v>236</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>13</v>
+      </c>
+      <c r="B298" t="s">
+        <v>5</v>
+      </c>
+      <c r="C298">
+        <v>236</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>13</v>
+      </c>
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299">
+        <v>236</v>
+      </c>
+      <c r="D299">
+        <v>1</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>14</v>
+      </c>
+      <c r="B300" t="s">
+        <v>5</v>
+      </c>
+      <c r="C300">
+        <v>236</v>
+      </c>
+      <c r="D300">
+        <v>1</v>
+      </c>
+      <c r="E300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>14</v>
+      </c>
+      <c r="B301" t="s">
+        <v>6</v>
+      </c>
+      <c r="C301">
+        <v>236</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>15</v>
+      </c>
+      <c r="B302" t="s">
+        <v>5</v>
+      </c>
+      <c r="C302">
+        <v>236</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>15</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303">
+        <v>236</v>
+      </c>
+      <c r="D303">
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>16</v>
+      </c>
+      <c r="B304" t="s">
+        <v>5</v>
+      </c>
+      <c r="C304">
+        <v>236</v>
+      </c>
+      <c r="D304">
+        <v>3</v>
+      </c>
+      <c r="E304">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>16</v>
+      </c>
+      <c r="B305" t="s">
+        <v>6</v>
+      </c>
+      <c r="C305">
+        <v>236</v>
+      </c>
+      <c r="D305">
+        <v>2</v>
+      </c>
+      <c r="E305">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>17</v>
+      </c>
+      <c r="B306" t="s">
+        <v>5</v>
+      </c>
+      <c r="C306">
+        <v>236</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+      <c r="E306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>17</v>
+      </c>
+      <c r="B307" t="s">
+        <v>6</v>
+      </c>
+      <c r="C307">
+        <v>236</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>18</v>
+      </c>
+      <c r="B308" t="s">
+        <v>5</v>
+      </c>
+      <c r="C308">
+        <v>236</v>
+      </c>
+      <c r="D308">
+        <v>1</v>
+      </c>
+      <c r="E308">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>18</v>
+      </c>
+      <c r="B309" t="s">
+        <v>6</v>
+      </c>
+      <c r="C309">
+        <v>236</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+      <c r="E309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>19</v>
+      </c>
+      <c r="B310" t="s">
+        <v>5</v>
+      </c>
+      <c r="C310">
+        <v>236</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>19</v>
+      </c>
+      <c r="B311" t="s">
+        <v>6</v>
+      </c>
+      <c r="C311">
+        <v>236</v>
+      </c>
+      <c r="D311">
+        <v>2</v>
+      </c>
+      <c r="E311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>20</v>
+      </c>
+      <c r="B312" t="s">
+        <v>5</v>
+      </c>
+      <c r="C312">
+        <v>236</v>
+      </c>
+      <c r="D312">
+        <v>1</v>
+      </c>
+      <c r="E312">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>20</v>
+      </c>
+      <c r="B313" t="s">
+        <v>6</v>
+      </c>
+      <c r="C313">
+        <v>236</v>
+      </c>
+      <c r="D313">
+        <v>2</v>
+      </c>
+      <c r="E313">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>21</v>
+      </c>
+      <c r="B314" t="s">
+        <v>5</v>
+      </c>
+      <c r="C314">
+        <v>236</v>
+      </c>
+      <c r="D314">
+        <v>0</v>
+      </c>
+      <c r="E314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>21</v>
+      </c>
+      <c r="B315" t="s">
+        <v>6</v>
+      </c>
+      <c r="C315">
+        <v>236</v>
+      </c>
+      <c r="D315">
+        <v>6</v>
+      </c>
+      <c r="E315">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>22</v>
+      </c>
+      <c r="B316" t="s">
+        <v>5</v>
+      </c>
+      <c r="C316">
+        <v>236</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>22</v>
+      </c>
+      <c r="B317" t="s">
+        <v>6</v>
+      </c>
+      <c r="C317">
+        <v>236</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+      <c r="E317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>23</v>
+      </c>
+      <c r="B318" t="s">
+        <v>5</v>
+      </c>
+      <c r="C318">
+        <v>236</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>23</v>
+      </c>
+      <c r="B319" t="s">
+        <v>6</v>
+      </c>
+      <c r="C319">
+        <v>236</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>24</v>
+      </c>
+      <c r="B320" t="s">
+        <v>5</v>
+      </c>
+      <c r="C320">
+        <v>236</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>24</v>
+      </c>
+      <c r="B321" t="s">
+        <v>6</v>
+      </c>
+      <c r="C321">
+        <v>236</v>
+      </c>
+      <c r="D321">
+        <v>1</v>
+      </c>
+      <c r="E321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>25</v>
+      </c>
+      <c r="B322" t="s">
+        <v>5</v>
+      </c>
+      <c r="C322">
+        <v>236</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>25</v>
+      </c>
+      <c r="B323" t="s">
+        <v>6</v>
+      </c>
+      <c r="C323">
+        <v>236</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+      <c r="E323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>26</v>
+      </c>
+      <c r="B324" t="s">
+        <v>5</v>
+      </c>
+      <c r="C324">
+        <v>236</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+      <c r="E324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>26</v>
+      </c>
+      <c r="B325" t="s">
+        <v>6</v>
+      </c>
+      <c r="C325">
+        <v>236</v>
+      </c>
+      <c r="D325">
+        <v>0</v>
+      </c>
+      <c r="E325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>27</v>
+      </c>
+      <c r="B326" t="s">
+        <v>5</v>
+      </c>
+      <c r="C326">
+        <v>236</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+      <c r="E326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>27</v>
+      </c>
+      <c r="B327" t="s">
+        <v>6</v>
+      </c>
+      <c r="C327">
+        <v>236</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>28</v>
+      </c>
+      <c r="B328" t="s">
+        <v>5</v>
+      </c>
+      <c r="C328">
+        <v>236</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>28</v>
+      </c>
+      <c r="B329" t="s">
+        <v>6</v>
+      </c>
+      <c r="C329">
+        <v>236</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>29</v>
+      </c>
+      <c r="B330" t="s">
+        <v>5</v>
+      </c>
+      <c r="C330">
+        <v>236</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>29</v>
+      </c>
+      <c r="B331" t="s">
+        <v>6</v>
+      </c>
+      <c r="C331">
+        <v>236</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+      <c r="E331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>30</v>
+      </c>
+      <c r="B332" t="s">
+        <v>5</v>
+      </c>
+      <c r="C332">
+        <v>236</v>
+      </c>
+      <c r="D332">
+        <v>4</v>
+      </c>
+      <c r="E332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>30</v>
+      </c>
+      <c r="B333" t="s">
+        <v>6</v>
+      </c>
+      <c r="C333">
+        <v>236</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>31</v>
+      </c>
+      <c r="B334" t="s">
+        <v>5</v>
+      </c>
+      <c r="C334">
+        <v>236</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+      <c r="E334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>31</v>
+      </c>
+      <c r="B335" t="s">
+        <v>6</v>
+      </c>
+      <c r="C335">
+        <v>236</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>32</v>
+      </c>
+      <c r="B336" t="s">
+        <v>5</v>
+      </c>
+      <c r="C336">
+        <v>236</v>
+      </c>
+      <c r="D336">
+        <v>2</v>
+      </c>
+      <c r="E336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>32</v>
+      </c>
+      <c r="B337" t="s">
+        <v>6</v>
+      </c>
+      <c r="C337">
+        <v>236</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>33</v>
+      </c>
+      <c r="B338" t="s">
+        <v>5</v>
+      </c>
+      <c r="C338">
+        <v>236</v>
+      </c>
+      <c r="D338">
+        <v>2</v>
+      </c>
+      <c r="E338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <v>33</v>
+      </c>
+      <c r="B339" t="s">
+        <v>6</v>
+      </c>
+      <c r="C339">
+        <v>236</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>34</v>
+      </c>
+      <c r="B340" t="s">
+        <v>5</v>
+      </c>
+      <c r="C340">
+        <v>236</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>34</v>
+      </c>
+      <c r="B341" t="s">
+        <v>6</v>
+      </c>
+      <c r="C341">
+        <v>236</v>
+      </c>
+      <c r="D341">
+        <v>1</v>
+      </c>
+      <c r="E341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>1</v>
+      </c>
+      <c r="B342" t="s">
+        <v>5</v>
+      </c>
+      <c r="C342">
+        <v>244</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+      <c r="E342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>1</v>
+      </c>
+      <c r="B343" t="s">
+        <v>6</v>
+      </c>
+      <c r="C343">
+        <v>244</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+      <c r="E343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>2</v>
+      </c>
+      <c r="B344" t="s">
+        <v>5</v>
+      </c>
+      <c r="C344">
+        <v>244</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+      <c r="E344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>2</v>
+      </c>
+      <c r="B345" t="s">
+        <v>6</v>
+      </c>
+      <c r="C345">
+        <v>244</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+      <c r="E345">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>3</v>
+      </c>
+      <c r="B346" t="s">
+        <v>5</v>
+      </c>
+      <c r="C346">
+        <v>244</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+      <c r="E346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <v>3</v>
+      </c>
+      <c r="B347" t="s">
+        <v>6</v>
+      </c>
+      <c r="C347">
+        <v>244</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+      <c r="E347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <v>4</v>
+      </c>
+      <c r="B348" t="s">
+        <v>5</v>
+      </c>
+      <c r="C348">
+        <v>244</v>
+      </c>
+      <c r="D348">
+        <v>2</v>
+      </c>
+      <c r="E348">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <v>4</v>
+      </c>
+      <c r="B349" t="s">
+        <v>6</v>
+      </c>
+      <c r="C349">
+        <v>244</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+      <c r="E349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <v>5</v>
+      </c>
+      <c r="B350" t="s">
+        <v>5</v>
+      </c>
+      <c r="C350">
+        <v>244</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+      <c r="E350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <v>5</v>
+      </c>
+      <c r="B351" t="s">
+        <v>6</v>
+      </c>
+      <c r="C351">
+        <v>244</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+      <c r="E351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A352">
+        <v>6</v>
+      </c>
+      <c r="B352" t="s">
+        <v>5</v>
+      </c>
+      <c r="C352">
+        <v>244</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A353">
+        <v>6</v>
+      </c>
+      <c r="B353" t="s">
+        <v>6</v>
+      </c>
+      <c r="C353">
+        <v>244</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+      <c r="E353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A354">
+        <v>7</v>
+      </c>
+      <c r="B354" t="s">
+        <v>5</v>
+      </c>
+      <c r="C354">
+        <v>244</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+      <c r="E354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A355">
+        <v>7</v>
+      </c>
+      <c r="B355" t="s">
+        <v>6</v>
+      </c>
+      <c r="C355">
+        <v>244</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+      <c r="E355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A356">
+        <v>8</v>
+      </c>
+      <c r="B356" t="s">
+        <v>5</v>
+      </c>
+      <c r="C356">
+        <v>244</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>8</v>
+      </c>
+      <c r="B357" t="s">
+        <v>6</v>
+      </c>
+      <c r="C357">
+        <v>244</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <v>9</v>
+      </c>
+      <c r="B358" t="s">
+        <v>5</v>
+      </c>
+      <c r="C358">
+        <v>244</v>
+      </c>
+      <c r="D358">
+        <v>1</v>
+      </c>
+      <c r="E358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <v>9</v>
+      </c>
+      <c r="B359" t="s">
+        <v>6</v>
+      </c>
+      <c r="C359">
+        <v>244</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+      <c r="E359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <v>10</v>
+      </c>
+      <c r="B360" t="s">
+        <v>5</v>
+      </c>
+      <c r="C360">
+        <v>244</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <v>10</v>
+      </c>
+      <c r="B361" t="s">
+        <v>6</v>
+      </c>
+      <c r="C361">
+        <v>244</v>
+      </c>
+      <c r="D361">
+        <v>1</v>
+      </c>
+      <c r="E361">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>11</v>
+      </c>
+      <c r="B362" t="s">
+        <v>5</v>
+      </c>
+      <c r="C362">
+        <v>244</v>
+      </c>
+      <c r="D362">
+        <v>1</v>
+      </c>
+      <c r="E362">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <v>11</v>
+      </c>
+      <c r="B363" t="s">
+        <v>6</v>
+      </c>
+      <c r="C363">
+        <v>244</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <v>12</v>
+      </c>
+      <c r="B364" t="s">
+        <v>5</v>
+      </c>
+      <c r="C364">
+        <v>244</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <v>12</v>
+      </c>
+      <c r="B365" t="s">
+        <v>6</v>
+      </c>
+      <c r="C365">
+        <v>244</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <v>13</v>
+      </c>
+      <c r="B366" t="s">
+        <v>5</v>
+      </c>
+      <c r="C366">
+        <v>244</v>
+      </c>
+      <c r="D366">
+        <v>1</v>
+      </c>
+      <c r="E366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <v>13</v>
+      </c>
+      <c r="B367" t="s">
+        <v>6</v>
+      </c>
+      <c r="C367">
+        <v>244</v>
+      </c>
+      <c r="D367">
+        <v>1</v>
+      </c>
+      <c r="E367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <v>14</v>
+      </c>
+      <c r="B368" t="s">
+        <v>5</v>
+      </c>
+      <c r="C368">
+        <v>244</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>14</v>
+      </c>
+      <c r="B369" t="s">
+        <v>6</v>
+      </c>
+      <c r="C369">
+        <v>244</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>15</v>
+      </c>
+      <c r="B370" t="s">
+        <v>5</v>
+      </c>
+      <c r="C370">
+        <v>244</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>15</v>
+      </c>
+      <c r="B371" t="s">
+        <v>6</v>
+      </c>
+      <c r="C371">
+        <v>244</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>16</v>
+      </c>
+      <c r="B372" t="s">
+        <v>5</v>
+      </c>
+      <c r="C372">
+        <v>244</v>
+      </c>
+      <c r="D372">
+        <v>1</v>
+      </c>
+      <c r="E372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>16</v>
+      </c>
+      <c r="B373" t="s">
+        <v>6</v>
+      </c>
+      <c r="C373">
+        <v>244</v>
+      </c>
+      <c r="D373">
+        <v>1</v>
+      </c>
+      <c r="E373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>17</v>
+      </c>
+      <c r="B374" t="s">
+        <v>5</v>
+      </c>
+      <c r="C374">
+        <v>244</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>17</v>
+      </c>
+      <c r="B375" t="s">
+        <v>6</v>
+      </c>
+      <c r="C375">
+        <v>244</v>
+      </c>
+      <c r="D375">
+        <v>3</v>
+      </c>
+      <c r="E375">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <v>18</v>
+      </c>
+      <c r="B376" t="s">
+        <v>5</v>
+      </c>
+      <c r="C376">
+        <v>244</v>
+      </c>
+      <c r="D376">
+        <v>1</v>
+      </c>
+      <c r="E376">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <v>18</v>
+      </c>
+      <c r="B377" t="s">
+        <v>6</v>
+      </c>
+      <c r="C377">
+        <v>244</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>19</v>
+      </c>
+      <c r="B378" t="s">
+        <v>5</v>
+      </c>
+      <c r="C378">
+        <v>244</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>19</v>
+      </c>
+      <c r="B379" t="s">
+        <v>6</v>
+      </c>
+      <c r="C379">
+        <v>244</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>20</v>
+      </c>
+      <c r="B380" t="s">
+        <v>5</v>
+      </c>
+      <c r="C380">
+        <v>244</v>
+      </c>
+      <c r="D380">
+        <v>2</v>
+      </c>
+      <c r="E380">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>20</v>
+      </c>
+      <c r="B381" t="s">
+        <v>6</v>
+      </c>
+      <c r="C381">
+        <v>244</v>
+      </c>
+      <c r="D381">
+        <v>3</v>
+      </c>
+      <c r="E381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>21</v>
+      </c>
+      <c r="B382" t="s">
+        <v>5</v>
+      </c>
+      <c r="C382">
+        <v>244</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>21</v>
+      </c>
+      <c r="B383" t="s">
+        <v>6</v>
+      </c>
+      <c r="C383">
+        <v>244</v>
+      </c>
+      <c r="D383">
+        <v>1</v>
+      </c>
+      <c r="E383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>22</v>
+      </c>
+      <c r="B384" t="s">
+        <v>5</v>
+      </c>
+      <c r="C384">
+        <v>244</v>
+      </c>
+      <c r="D384">
+        <v>0</v>
+      </c>
+      <c r="E384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>22</v>
+      </c>
+      <c r="B385" t="s">
+        <v>6</v>
+      </c>
+      <c r="C385">
+        <v>244</v>
+      </c>
+      <c r="D385">
+        <v>0</v>
+      </c>
+      <c r="E385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>23</v>
+      </c>
+      <c r="B386" t="s">
+        <v>5</v>
+      </c>
+      <c r="C386">
+        <v>244</v>
+      </c>
+      <c r="D386">
+        <v>1</v>
+      </c>
+      <c r="E386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>23</v>
+      </c>
+      <c r="B387" t="s">
+        <v>6</v>
+      </c>
+      <c r="C387">
+        <v>244</v>
+      </c>
+      <c r="D387">
+        <v>1</v>
+      </c>
+      <c r="E387">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>24</v>
+      </c>
+      <c r="B388" t="s">
+        <v>5</v>
+      </c>
+      <c r="C388">
+        <v>244</v>
+      </c>
+      <c r="D388">
+        <v>0</v>
+      </c>
+      <c r="E388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>24</v>
+      </c>
+      <c r="B389" t="s">
+        <v>6</v>
+      </c>
+      <c r="C389">
+        <v>244</v>
+      </c>
+      <c r="D389">
+        <v>0</v>
+      </c>
+      <c r="E389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>25</v>
+      </c>
+      <c r="B390" t="s">
+        <v>5</v>
+      </c>
+      <c r="C390">
+        <v>244</v>
+      </c>
+      <c r="D390">
+        <v>0</v>
+      </c>
+      <c r="E390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>25</v>
+      </c>
+      <c r="B391" t="s">
+        <v>6</v>
+      </c>
+      <c r="C391">
+        <v>244</v>
+      </c>
+      <c r="D391">
+        <v>0</v>
+      </c>
+      <c r="E391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>26</v>
+      </c>
+      <c r="B392" t="s">
+        <v>5</v>
+      </c>
+      <c r="C392">
+        <v>244</v>
+      </c>
+      <c r="D392">
+        <v>0</v>
+      </c>
+      <c r="E392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>26</v>
+      </c>
+      <c r="B393" t="s">
+        <v>6</v>
+      </c>
+      <c r="C393">
+        <v>244</v>
+      </c>
+      <c r="D393">
+        <v>0</v>
+      </c>
+      <c r="E393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>27</v>
+      </c>
+      <c r="B394" t="s">
+        <v>5</v>
+      </c>
+      <c r="C394">
+        <v>244</v>
+      </c>
+      <c r="D394">
+        <v>0</v>
+      </c>
+      <c r="E394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>27</v>
+      </c>
+      <c r="B395" t="s">
+        <v>6</v>
+      </c>
+      <c r="C395">
+        <v>244</v>
+      </c>
+      <c r="D395">
+        <v>0</v>
+      </c>
+      <c r="E395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>28</v>
+      </c>
+      <c r="B396" t="s">
+        <v>5</v>
+      </c>
+      <c r="C396">
+        <v>244</v>
+      </c>
+      <c r="D396">
+        <v>0</v>
+      </c>
+      <c r="E396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>28</v>
+      </c>
+      <c r="B397" t="s">
+        <v>6</v>
+      </c>
+      <c r="C397">
+        <v>244</v>
+      </c>
+      <c r="D397">
+        <v>0</v>
+      </c>
+      <c r="E397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>29</v>
+      </c>
+      <c r="B398" t="s">
+        <v>5</v>
+      </c>
+      <c r="C398">
+        <v>244</v>
+      </c>
+      <c r="D398">
+        <v>1</v>
+      </c>
+      <c r="E398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>29</v>
+      </c>
+      <c r="B399" t="s">
+        <v>6</v>
+      </c>
+      <c r="C399">
+        <v>244</v>
+      </c>
+      <c r="D399">
+        <v>0</v>
+      </c>
+      <c r="E399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>30</v>
+      </c>
+      <c r="B400" t="s">
+        <v>5</v>
+      </c>
+      <c r="C400">
+        <v>244</v>
+      </c>
+      <c r="D400">
+        <v>0</v>
+      </c>
+      <c r="E400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>30</v>
+      </c>
+      <c r="B401" t="s">
+        <v>6</v>
+      </c>
+      <c r="C401">
+        <v>244</v>
+      </c>
+      <c r="D401">
+        <v>0</v>
+      </c>
+      <c r="E401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>31</v>
+      </c>
+      <c r="B402" t="s">
+        <v>5</v>
+      </c>
+      <c r="C402">
+        <v>244</v>
+      </c>
+      <c r="D402">
+        <v>0</v>
+      </c>
+      <c r="E402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>31</v>
+      </c>
+      <c r="B403" t="s">
+        <v>6</v>
+      </c>
+      <c r="C403">
+        <v>244</v>
+      </c>
+      <c r="D403">
+        <v>0</v>
+      </c>
+      <c r="E403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>32</v>
+      </c>
+      <c r="B404" t="s">
+        <v>5</v>
+      </c>
+      <c r="C404">
+        <v>244</v>
+      </c>
+      <c r="D404">
+        <v>1</v>
+      </c>
+      <c r="E404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>32</v>
+      </c>
+      <c r="B405" t="s">
+        <v>6</v>
+      </c>
+      <c r="C405">
+        <v>244</v>
+      </c>
+      <c r="D405">
+        <v>0</v>
+      </c>
+      <c r="E405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>33</v>
+      </c>
+      <c r="B406" t="s">
+        <v>5</v>
+      </c>
+      <c r="C406">
+        <v>244</v>
+      </c>
+      <c r="D406">
+        <v>1</v>
+      </c>
+      <c r="E406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>33</v>
+      </c>
+      <c r="B407" t="s">
+        <v>6</v>
+      </c>
+      <c r="C407">
+        <v>244</v>
+      </c>
+      <c r="D407">
+        <v>0</v>
+      </c>
+      <c r="E407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>34</v>
+      </c>
+      <c r="B408" t="s">
+        <v>5</v>
+      </c>
+      <c r="C408">
+        <v>244</v>
+      </c>
+      <c r="D408">
+        <v>1</v>
+      </c>
+      <c r="E408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>34</v>
+      </c>
+      <c r="B409" t="s">
+        <v>6</v>
+      </c>
+      <c r="C409">
+        <v>244</v>
+      </c>
+      <c r="D409">
+        <v>1</v>
+      </c>
+      <c r="E409">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the data files for fly and pupae development with new data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/fly_part2.xlsx
+++ b/data/fitness_development/fly_part2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_13/data/fitness_development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_14/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED272A5-4B2B-254D-B2EA-C81B42521305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFD7433-D11C-B24E-A6FD-F115AB11E9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BB242E00-5CB3-A84F-BA7A-96A75344F1EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{BB242E00-5CB3-A84F-BA7A-96A75344F1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB267A-8CE1-0F4E-97AE-D44F1974EE08}">
-  <dimension ref="A1:E409"/>
+  <dimension ref="A1:E613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A387" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E409" sqref="E409"/>
+    <sheetView tabSelected="1" topLeftCell="A605" zoomScale="305" workbookViewId="0">
+      <selection activeCell="D614" sqref="D614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7392,6 +7392,3474 @@
         <v>0</v>
       </c>
     </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>1</v>
+      </c>
+      <c r="B410" t="s">
+        <v>5</v>
+      </c>
+      <c r="C410">
+        <v>260</v>
+      </c>
+      <c r="D410">
+        <v>1</v>
+      </c>
+      <c r="E410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>1</v>
+      </c>
+      <c r="B411" t="s">
+        <v>6</v>
+      </c>
+      <c r="C411">
+        <v>260</v>
+      </c>
+      <c r="D411">
+        <v>0</v>
+      </c>
+      <c r="E411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>2</v>
+      </c>
+      <c r="B412" t="s">
+        <v>5</v>
+      </c>
+      <c r="C412">
+        <v>260</v>
+      </c>
+      <c r="D412">
+        <v>1</v>
+      </c>
+      <c r="E412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>2</v>
+      </c>
+      <c r="B413" t="s">
+        <v>6</v>
+      </c>
+      <c r="C413">
+        <v>260</v>
+      </c>
+      <c r="D413">
+        <v>0</v>
+      </c>
+      <c r="E413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>3</v>
+      </c>
+      <c r="B414" t="s">
+        <v>5</v>
+      </c>
+      <c r="C414">
+        <v>260</v>
+      </c>
+      <c r="D414">
+        <v>0</v>
+      </c>
+      <c r="E414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>3</v>
+      </c>
+      <c r="B415" t="s">
+        <v>6</v>
+      </c>
+      <c r="C415">
+        <v>260</v>
+      </c>
+      <c r="D415">
+        <v>5</v>
+      </c>
+      <c r="E415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>4</v>
+      </c>
+      <c r="B416" t="s">
+        <v>5</v>
+      </c>
+      <c r="C416">
+        <v>260</v>
+      </c>
+      <c r="D416">
+        <v>0</v>
+      </c>
+      <c r="E416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>4</v>
+      </c>
+      <c r="B417" t="s">
+        <v>6</v>
+      </c>
+      <c r="C417">
+        <v>260</v>
+      </c>
+      <c r="D417">
+        <v>0</v>
+      </c>
+      <c r="E417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>5</v>
+      </c>
+      <c r="B418" t="s">
+        <v>5</v>
+      </c>
+      <c r="C418">
+        <v>260</v>
+      </c>
+      <c r="D418">
+        <v>0</v>
+      </c>
+      <c r="E418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>5</v>
+      </c>
+      <c r="B419" t="s">
+        <v>6</v>
+      </c>
+      <c r="C419">
+        <v>260</v>
+      </c>
+      <c r="D419">
+        <v>0</v>
+      </c>
+      <c r="E419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>6</v>
+      </c>
+      <c r="B420" t="s">
+        <v>5</v>
+      </c>
+      <c r="C420">
+        <v>260</v>
+      </c>
+      <c r="D420">
+        <v>1</v>
+      </c>
+      <c r="E420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>6</v>
+      </c>
+      <c r="B421" t="s">
+        <v>6</v>
+      </c>
+      <c r="C421">
+        <v>260</v>
+      </c>
+      <c r="D421">
+        <v>0</v>
+      </c>
+      <c r="E421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>7</v>
+      </c>
+      <c r="B422" t="s">
+        <v>5</v>
+      </c>
+      <c r="C422">
+        <v>260</v>
+      </c>
+      <c r="D422">
+        <v>2</v>
+      </c>
+      <c r="E422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>7</v>
+      </c>
+      <c r="B423" t="s">
+        <v>6</v>
+      </c>
+      <c r="C423">
+        <v>260</v>
+      </c>
+      <c r="D423">
+        <v>0</v>
+      </c>
+      <c r="E423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>8</v>
+      </c>
+      <c r="B424" t="s">
+        <v>5</v>
+      </c>
+      <c r="C424">
+        <v>260</v>
+      </c>
+      <c r="D424">
+        <v>0</v>
+      </c>
+      <c r="E424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>8</v>
+      </c>
+      <c r="B425" t="s">
+        <v>6</v>
+      </c>
+      <c r="C425">
+        <v>260</v>
+      </c>
+      <c r="D425">
+        <v>0</v>
+      </c>
+      <c r="E425">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>9</v>
+      </c>
+      <c r="B426" t="s">
+        <v>5</v>
+      </c>
+      <c r="C426">
+        <v>260</v>
+      </c>
+      <c r="D426">
+        <v>0</v>
+      </c>
+      <c r="E426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>9</v>
+      </c>
+      <c r="B427" t="s">
+        <v>6</v>
+      </c>
+      <c r="C427">
+        <v>260</v>
+      </c>
+      <c r="D427">
+        <v>1</v>
+      </c>
+      <c r="E427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>10</v>
+      </c>
+      <c r="B428" t="s">
+        <v>5</v>
+      </c>
+      <c r="C428">
+        <v>260</v>
+      </c>
+      <c r="D428">
+        <v>0</v>
+      </c>
+      <c r="E428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>10</v>
+      </c>
+      <c r="B429" t="s">
+        <v>6</v>
+      </c>
+      <c r="C429">
+        <v>260</v>
+      </c>
+      <c r="D429">
+        <v>1</v>
+      </c>
+      <c r="E429">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>11</v>
+      </c>
+      <c r="B430" t="s">
+        <v>5</v>
+      </c>
+      <c r="C430">
+        <v>260</v>
+      </c>
+      <c r="D430">
+        <v>0</v>
+      </c>
+      <c r="E430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>11</v>
+      </c>
+      <c r="B431" t="s">
+        <v>6</v>
+      </c>
+      <c r="C431">
+        <v>260</v>
+      </c>
+      <c r="D431">
+        <v>1</v>
+      </c>
+      <c r="E431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>12</v>
+      </c>
+      <c r="B432" t="s">
+        <v>5</v>
+      </c>
+      <c r="C432">
+        <v>260</v>
+      </c>
+      <c r="D432">
+        <v>0</v>
+      </c>
+      <c r="E432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>12</v>
+      </c>
+      <c r="B433" t="s">
+        <v>6</v>
+      </c>
+      <c r="C433">
+        <v>260</v>
+      </c>
+      <c r="D433">
+        <v>0</v>
+      </c>
+      <c r="E433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>13</v>
+      </c>
+      <c r="B434" t="s">
+        <v>5</v>
+      </c>
+      <c r="C434">
+        <v>260</v>
+      </c>
+      <c r="D434">
+        <v>1</v>
+      </c>
+      <c r="E434">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>13</v>
+      </c>
+      <c r="B435" t="s">
+        <v>6</v>
+      </c>
+      <c r="C435">
+        <v>260</v>
+      </c>
+      <c r="D435">
+        <v>2</v>
+      </c>
+      <c r="E435">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>14</v>
+      </c>
+      <c r="B436" t="s">
+        <v>5</v>
+      </c>
+      <c r="C436">
+        <v>260</v>
+      </c>
+      <c r="D436">
+        <v>0</v>
+      </c>
+      <c r="E436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>14</v>
+      </c>
+      <c r="B437" t="s">
+        <v>6</v>
+      </c>
+      <c r="C437">
+        <v>260</v>
+      </c>
+      <c r="D437">
+        <v>0</v>
+      </c>
+      <c r="E437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>15</v>
+      </c>
+      <c r="B438" t="s">
+        <v>5</v>
+      </c>
+      <c r="C438">
+        <v>260</v>
+      </c>
+      <c r="D438">
+        <v>4</v>
+      </c>
+      <c r="E438">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>15</v>
+      </c>
+      <c r="B439" t="s">
+        <v>6</v>
+      </c>
+      <c r="C439">
+        <v>260</v>
+      </c>
+      <c r="D439">
+        <v>0</v>
+      </c>
+      <c r="E439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>16</v>
+      </c>
+      <c r="B440" t="s">
+        <v>5</v>
+      </c>
+      <c r="C440">
+        <v>260</v>
+      </c>
+      <c r="D440">
+        <v>0</v>
+      </c>
+      <c r="E440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>16</v>
+      </c>
+      <c r="B441" t="s">
+        <v>6</v>
+      </c>
+      <c r="C441">
+        <v>260</v>
+      </c>
+      <c r="D441">
+        <v>1</v>
+      </c>
+      <c r="E441">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>17</v>
+      </c>
+      <c r="B442" t="s">
+        <v>5</v>
+      </c>
+      <c r="C442">
+        <v>260</v>
+      </c>
+      <c r="D442">
+        <v>0</v>
+      </c>
+      <c r="E442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>17</v>
+      </c>
+      <c r="B443" t="s">
+        <v>6</v>
+      </c>
+      <c r="C443">
+        <v>260</v>
+      </c>
+      <c r="D443">
+        <v>0</v>
+      </c>
+      <c r="E443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>18</v>
+      </c>
+      <c r="B444" t="s">
+        <v>5</v>
+      </c>
+      <c r="C444">
+        <v>260</v>
+      </c>
+      <c r="D444">
+        <v>0</v>
+      </c>
+      <c r="E444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>18</v>
+      </c>
+      <c r="B445" t="s">
+        <v>6</v>
+      </c>
+      <c r="C445">
+        <v>260</v>
+      </c>
+      <c r="D445">
+        <v>0</v>
+      </c>
+      <c r="E445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>19</v>
+      </c>
+      <c r="B446" t="s">
+        <v>5</v>
+      </c>
+      <c r="C446">
+        <v>260</v>
+      </c>
+      <c r="D446">
+        <v>1</v>
+      </c>
+      <c r="E446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>19</v>
+      </c>
+      <c r="B447" t="s">
+        <v>6</v>
+      </c>
+      <c r="C447">
+        <v>260</v>
+      </c>
+      <c r="D447">
+        <v>0</v>
+      </c>
+      <c r="E447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>20</v>
+      </c>
+      <c r="B448" t="s">
+        <v>5</v>
+      </c>
+      <c r="C448">
+        <v>260</v>
+      </c>
+      <c r="D448">
+        <v>0</v>
+      </c>
+      <c r="E448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>20</v>
+      </c>
+      <c r="B449" t="s">
+        <v>6</v>
+      </c>
+      <c r="C449">
+        <v>260</v>
+      </c>
+      <c r="D449">
+        <v>0</v>
+      </c>
+      <c r="E449">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>21</v>
+      </c>
+      <c r="B450" t="s">
+        <v>5</v>
+      </c>
+      <c r="C450">
+        <v>260</v>
+      </c>
+      <c r="D450">
+        <v>0</v>
+      </c>
+      <c r="E450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>21</v>
+      </c>
+      <c r="B451" t="s">
+        <v>6</v>
+      </c>
+      <c r="C451">
+        <v>260</v>
+      </c>
+      <c r="D451">
+        <v>0</v>
+      </c>
+      <c r="E451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>22</v>
+      </c>
+      <c r="B452" t="s">
+        <v>5</v>
+      </c>
+      <c r="C452">
+        <v>260</v>
+      </c>
+      <c r="D452">
+        <v>0</v>
+      </c>
+      <c r="E452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>22</v>
+      </c>
+      <c r="B453" t="s">
+        <v>6</v>
+      </c>
+      <c r="C453">
+        <v>260</v>
+      </c>
+      <c r="D453">
+        <v>0</v>
+      </c>
+      <c r="E453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>23</v>
+      </c>
+      <c r="B454" t="s">
+        <v>5</v>
+      </c>
+      <c r="C454">
+        <v>260</v>
+      </c>
+      <c r="D454">
+        <v>0</v>
+      </c>
+      <c r="E454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>23</v>
+      </c>
+      <c r="B455" t="s">
+        <v>6</v>
+      </c>
+      <c r="C455">
+        <v>260</v>
+      </c>
+      <c r="D455">
+        <v>0</v>
+      </c>
+      <c r="E455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>24</v>
+      </c>
+      <c r="B456" t="s">
+        <v>5</v>
+      </c>
+      <c r="C456">
+        <v>260</v>
+      </c>
+      <c r="D456">
+        <v>0</v>
+      </c>
+      <c r="E456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>24</v>
+      </c>
+      <c r="B457" t="s">
+        <v>6</v>
+      </c>
+      <c r="C457">
+        <v>260</v>
+      </c>
+      <c r="D457">
+        <v>0</v>
+      </c>
+      <c r="E457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>25</v>
+      </c>
+      <c r="B458" t="s">
+        <v>5</v>
+      </c>
+      <c r="C458">
+        <v>260</v>
+      </c>
+      <c r="D458">
+        <v>0</v>
+      </c>
+      <c r="E458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>25</v>
+      </c>
+      <c r="B459" t="s">
+        <v>6</v>
+      </c>
+      <c r="C459">
+        <v>260</v>
+      </c>
+      <c r="D459">
+        <v>0</v>
+      </c>
+      <c r="E459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>26</v>
+      </c>
+      <c r="B460" t="s">
+        <v>5</v>
+      </c>
+      <c r="C460">
+        <v>260</v>
+      </c>
+      <c r="D460">
+        <v>0</v>
+      </c>
+      <c r="E460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>26</v>
+      </c>
+      <c r="B461" t="s">
+        <v>6</v>
+      </c>
+      <c r="C461">
+        <v>260</v>
+      </c>
+      <c r="D461">
+        <v>1</v>
+      </c>
+      <c r="E461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>27</v>
+      </c>
+      <c r="B462" t="s">
+        <v>5</v>
+      </c>
+      <c r="C462">
+        <v>260</v>
+      </c>
+      <c r="D462">
+        <v>0</v>
+      </c>
+      <c r="E462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>27</v>
+      </c>
+      <c r="B463" t="s">
+        <v>6</v>
+      </c>
+      <c r="C463">
+        <v>260</v>
+      </c>
+      <c r="D463">
+        <v>0</v>
+      </c>
+      <c r="E463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>28</v>
+      </c>
+      <c r="B464" t="s">
+        <v>5</v>
+      </c>
+      <c r="C464">
+        <v>260</v>
+      </c>
+      <c r="D464">
+        <v>0</v>
+      </c>
+      <c r="E464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>28</v>
+      </c>
+      <c r="B465" t="s">
+        <v>6</v>
+      </c>
+      <c r="C465">
+        <v>260</v>
+      </c>
+      <c r="D465">
+        <v>3</v>
+      </c>
+      <c r="E465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>29</v>
+      </c>
+      <c r="B466" t="s">
+        <v>5</v>
+      </c>
+      <c r="C466">
+        <v>260</v>
+      </c>
+      <c r="D466">
+        <v>0</v>
+      </c>
+      <c r="E466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>29</v>
+      </c>
+      <c r="B467" t="s">
+        <v>6</v>
+      </c>
+      <c r="C467">
+        <v>260</v>
+      </c>
+      <c r="D467">
+        <v>0</v>
+      </c>
+      <c r="E467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>30</v>
+      </c>
+      <c r="B468" t="s">
+        <v>5</v>
+      </c>
+      <c r="C468">
+        <v>260</v>
+      </c>
+      <c r="D468">
+        <v>0</v>
+      </c>
+      <c r="E468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>30</v>
+      </c>
+      <c r="B469" t="s">
+        <v>6</v>
+      </c>
+      <c r="C469">
+        <v>260</v>
+      </c>
+      <c r="D469">
+        <v>1</v>
+      </c>
+      <c r="E469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>31</v>
+      </c>
+      <c r="B470" t="s">
+        <v>5</v>
+      </c>
+      <c r="C470">
+        <v>260</v>
+      </c>
+      <c r="D470">
+        <v>1</v>
+      </c>
+      <c r="E470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>31</v>
+      </c>
+      <c r="B471" t="s">
+        <v>6</v>
+      </c>
+      <c r="C471">
+        <v>260</v>
+      </c>
+      <c r="D471">
+        <v>0</v>
+      </c>
+      <c r="E471">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>32</v>
+      </c>
+      <c r="B472" t="s">
+        <v>5</v>
+      </c>
+      <c r="C472">
+        <v>260</v>
+      </c>
+      <c r="D472">
+        <v>3</v>
+      </c>
+      <c r="E472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>32</v>
+      </c>
+      <c r="B473" t="s">
+        <v>6</v>
+      </c>
+      <c r="C473">
+        <v>260</v>
+      </c>
+      <c r="D473">
+        <v>0</v>
+      </c>
+      <c r="E473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>33</v>
+      </c>
+      <c r="B474" t="s">
+        <v>5</v>
+      </c>
+      <c r="C474">
+        <v>260</v>
+      </c>
+      <c r="D474">
+        <v>0</v>
+      </c>
+      <c r="E474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>33</v>
+      </c>
+      <c r="B475" t="s">
+        <v>6</v>
+      </c>
+      <c r="C475">
+        <v>260</v>
+      </c>
+      <c r="D475">
+        <v>0</v>
+      </c>
+      <c r="E475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>34</v>
+      </c>
+      <c r="B476" t="s">
+        <v>5</v>
+      </c>
+      <c r="C476">
+        <v>260</v>
+      </c>
+      <c r="D476">
+        <v>1</v>
+      </c>
+      <c r="E476">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>34</v>
+      </c>
+      <c r="B477" t="s">
+        <v>6</v>
+      </c>
+      <c r="C477">
+        <v>260</v>
+      </c>
+      <c r="D477">
+        <v>0</v>
+      </c>
+      <c r="E477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>1</v>
+      </c>
+      <c r="B478" t="s">
+        <v>5</v>
+      </c>
+      <c r="C478">
+        <v>269</v>
+      </c>
+      <c r="D478">
+        <v>0</v>
+      </c>
+      <c r="E478">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>1</v>
+      </c>
+      <c r="B479" t="s">
+        <v>6</v>
+      </c>
+      <c r="C479">
+        <v>269</v>
+      </c>
+      <c r="D479">
+        <v>0</v>
+      </c>
+      <c r="E479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>2</v>
+      </c>
+      <c r="B480" t="s">
+        <v>5</v>
+      </c>
+      <c r="C480">
+        <v>269</v>
+      </c>
+      <c r="D480">
+        <v>1</v>
+      </c>
+      <c r="E480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>2</v>
+      </c>
+      <c r="B481" t="s">
+        <v>6</v>
+      </c>
+      <c r="C481">
+        <v>269</v>
+      </c>
+      <c r="D481">
+        <v>1</v>
+      </c>
+      <c r="E481">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <v>3</v>
+      </c>
+      <c r="B482" t="s">
+        <v>5</v>
+      </c>
+      <c r="C482">
+        <v>269</v>
+      </c>
+      <c r="D482">
+        <v>0</v>
+      </c>
+      <c r="E482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>3</v>
+      </c>
+      <c r="B483" t="s">
+        <v>6</v>
+      </c>
+      <c r="C483">
+        <v>269</v>
+      </c>
+      <c r="D483">
+        <v>2</v>
+      </c>
+      <c r="E483">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>4</v>
+      </c>
+      <c r="B484" t="s">
+        <v>5</v>
+      </c>
+      <c r="C484">
+        <v>269</v>
+      </c>
+      <c r="D484">
+        <v>0</v>
+      </c>
+      <c r="E484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>4</v>
+      </c>
+      <c r="B485" t="s">
+        <v>6</v>
+      </c>
+      <c r="C485">
+        <v>269</v>
+      </c>
+      <c r="D485">
+        <v>0</v>
+      </c>
+      <c r="E485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>5</v>
+      </c>
+      <c r="B486" t="s">
+        <v>5</v>
+      </c>
+      <c r="C486">
+        <v>269</v>
+      </c>
+      <c r="D486">
+        <v>0</v>
+      </c>
+      <c r="E486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>5</v>
+      </c>
+      <c r="B487" t="s">
+        <v>6</v>
+      </c>
+      <c r="C487">
+        <v>269</v>
+      </c>
+      <c r="D487">
+        <v>1</v>
+      </c>
+      <c r="E487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>6</v>
+      </c>
+      <c r="B488" t="s">
+        <v>5</v>
+      </c>
+      <c r="C488">
+        <v>269</v>
+      </c>
+      <c r="D488">
+        <v>2</v>
+      </c>
+      <c r="E488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <v>6</v>
+      </c>
+      <c r="B489" t="s">
+        <v>6</v>
+      </c>
+      <c r="C489">
+        <v>269</v>
+      </c>
+      <c r="D489">
+        <v>0</v>
+      </c>
+      <c r="E489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>7</v>
+      </c>
+      <c r="B490" t="s">
+        <v>5</v>
+      </c>
+      <c r="C490">
+        <v>269</v>
+      </c>
+      <c r="D490">
+        <v>1</v>
+      </c>
+      <c r="E490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>7</v>
+      </c>
+      <c r="B491" t="s">
+        <v>6</v>
+      </c>
+      <c r="C491">
+        <v>269</v>
+      </c>
+      <c r="D491">
+        <v>0</v>
+      </c>
+      <c r="E491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>8</v>
+      </c>
+      <c r="B492" t="s">
+        <v>5</v>
+      </c>
+      <c r="C492">
+        <v>269</v>
+      </c>
+      <c r="D492">
+        <v>0</v>
+      </c>
+      <c r="E492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>8</v>
+      </c>
+      <c r="B493" t="s">
+        <v>6</v>
+      </c>
+      <c r="C493">
+        <v>269</v>
+      </c>
+      <c r="D493">
+        <v>5</v>
+      </c>
+      <c r="E493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>9</v>
+      </c>
+      <c r="B494" t="s">
+        <v>5</v>
+      </c>
+      <c r="C494">
+        <v>269</v>
+      </c>
+      <c r="D494">
+        <v>2</v>
+      </c>
+      <c r="E494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>9</v>
+      </c>
+      <c r="B495" t="s">
+        <v>6</v>
+      </c>
+      <c r="C495">
+        <v>269</v>
+      </c>
+      <c r="D495">
+        <v>1</v>
+      </c>
+      <c r="E495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <v>10</v>
+      </c>
+      <c r="B496" t="s">
+        <v>5</v>
+      </c>
+      <c r="C496">
+        <v>269</v>
+      </c>
+      <c r="D496">
+        <v>0</v>
+      </c>
+      <c r="E496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <v>10</v>
+      </c>
+      <c r="B497" t="s">
+        <v>6</v>
+      </c>
+      <c r="C497">
+        <v>269</v>
+      </c>
+      <c r="D497">
+        <v>5</v>
+      </c>
+      <c r="E497">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <v>11</v>
+      </c>
+      <c r="B498" t="s">
+        <v>5</v>
+      </c>
+      <c r="C498">
+        <v>269</v>
+      </c>
+      <c r="D498">
+        <v>0</v>
+      </c>
+      <c r="E498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <v>11</v>
+      </c>
+      <c r="B499" t="s">
+        <v>6</v>
+      </c>
+      <c r="C499">
+        <v>269</v>
+      </c>
+      <c r="D499">
+        <v>0</v>
+      </c>
+      <c r="E499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <v>12</v>
+      </c>
+      <c r="B500" t="s">
+        <v>5</v>
+      </c>
+      <c r="C500">
+        <v>269</v>
+      </c>
+      <c r="D500">
+        <v>0</v>
+      </c>
+      <c r="E500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <v>12</v>
+      </c>
+      <c r="B501" t="s">
+        <v>6</v>
+      </c>
+      <c r="C501">
+        <v>269</v>
+      </c>
+      <c r="D501">
+        <v>0</v>
+      </c>
+      <c r="E501">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>13</v>
+      </c>
+      <c r="B502" t="s">
+        <v>5</v>
+      </c>
+      <c r="C502">
+        <v>269</v>
+      </c>
+      <c r="D502">
+        <v>3</v>
+      </c>
+      <c r="E502">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <v>13</v>
+      </c>
+      <c r="B503" t="s">
+        <v>6</v>
+      </c>
+      <c r="C503">
+        <v>269</v>
+      </c>
+      <c r="D503">
+        <v>3</v>
+      </c>
+      <c r="E503">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>14</v>
+      </c>
+      <c r="B504" t="s">
+        <v>5</v>
+      </c>
+      <c r="C504">
+        <v>269</v>
+      </c>
+      <c r="D504">
+        <v>2</v>
+      </c>
+      <c r="E504">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>14</v>
+      </c>
+      <c r="B505" t="s">
+        <v>6</v>
+      </c>
+      <c r="C505">
+        <v>269</v>
+      </c>
+      <c r="D505">
+        <v>1</v>
+      </c>
+      <c r="E505">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>15</v>
+      </c>
+      <c r="B506" t="s">
+        <v>5</v>
+      </c>
+      <c r="C506">
+        <v>269</v>
+      </c>
+      <c r="D506">
+        <v>0</v>
+      </c>
+      <c r="E506">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>15</v>
+      </c>
+      <c r="B507" t="s">
+        <v>6</v>
+      </c>
+      <c r="C507">
+        <v>269</v>
+      </c>
+      <c r="D507">
+        <v>0</v>
+      </c>
+      <c r="E507">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>16</v>
+      </c>
+      <c r="B508" t="s">
+        <v>5</v>
+      </c>
+      <c r="C508">
+        <v>269</v>
+      </c>
+      <c r="D508">
+        <v>1</v>
+      </c>
+      <c r="E508">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <v>16</v>
+      </c>
+      <c r="B509" t="s">
+        <v>6</v>
+      </c>
+      <c r="C509">
+        <v>269</v>
+      </c>
+      <c r="D509">
+        <v>1</v>
+      </c>
+      <c r="E509">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <v>17</v>
+      </c>
+      <c r="B510" t="s">
+        <v>5</v>
+      </c>
+      <c r="C510">
+        <v>269</v>
+      </c>
+      <c r="D510">
+        <v>2</v>
+      </c>
+      <c r="E510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <v>17</v>
+      </c>
+      <c r="B511" t="s">
+        <v>6</v>
+      </c>
+      <c r="C511">
+        <v>269</v>
+      </c>
+      <c r="D511">
+        <v>0</v>
+      </c>
+      <c r="E511">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <v>18</v>
+      </c>
+      <c r="B512" t="s">
+        <v>5</v>
+      </c>
+      <c r="C512">
+        <v>269</v>
+      </c>
+      <c r="D512">
+        <v>0</v>
+      </c>
+      <c r="E512">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A513">
+        <v>18</v>
+      </c>
+      <c r="B513" t="s">
+        <v>6</v>
+      </c>
+      <c r="C513">
+        <v>269</v>
+      </c>
+      <c r="D513">
+        <v>1</v>
+      </c>
+      <c r="E513">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <v>19</v>
+      </c>
+      <c r="B514" t="s">
+        <v>5</v>
+      </c>
+      <c r="C514">
+        <v>269</v>
+      </c>
+      <c r="D514">
+        <v>1</v>
+      </c>
+      <c r="E514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <v>19</v>
+      </c>
+      <c r="B515" t="s">
+        <v>6</v>
+      </c>
+      <c r="C515">
+        <v>269</v>
+      </c>
+      <c r="D515">
+        <v>2</v>
+      </c>
+      <c r="E515">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <v>20</v>
+      </c>
+      <c r="B516" t="s">
+        <v>5</v>
+      </c>
+      <c r="C516">
+        <v>269</v>
+      </c>
+      <c r="D516">
+        <v>4</v>
+      </c>
+      <c r="E516">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <v>20</v>
+      </c>
+      <c r="B517" t="s">
+        <v>6</v>
+      </c>
+      <c r="C517">
+        <v>269</v>
+      </c>
+      <c r="D517">
+        <v>0</v>
+      </c>
+      <c r="E517">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <v>21</v>
+      </c>
+      <c r="B518" t="s">
+        <v>5</v>
+      </c>
+      <c r="C518">
+        <v>269</v>
+      </c>
+      <c r="D518">
+        <v>0</v>
+      </c>
+      <c r="E518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <v>21</v>
+      </c>
+      <c r="B519" t="s">
+        <v>6</v>
+      </c>
+      <c r="C519">
+        <v>269</v>
+      </c>
+      <c r="D519">
+        <v>0</v>
+      </c>
+      <c r="E519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <v>22</v>
+      </c>
+      <c r="B520" t="s">
+        <v>5</v>
+      </c>
+      <c r="C520">
+        <v>269</v>
+      </c>
+      <c r="D520">
+        <v>0</v>
+      </c>
+      <c r="E520">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A521">
+        <v>22</v>
+      </c>
+      <c r="B521" t="s">
+        <v>6</v>
+      </c>
+      <c r="C521">
+        <v>269</v>
+      </c>
+      <c r="D521">
+        <v>0</v>
+      </c>
+      <c r="E521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A522">
+        <v>23</v>
+      </c>
+      <c r="B522" t="s">
+        <v>5</v>
+      </c>
+      <c r="C522">
+        <v>269</v>
+      </c>
+      <c r="D522">
+        <v>0</v>
+      </c>
+      <c r="E522">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A523">
+        <v>23</v>
+      </c>
+      <c r="B523" t="s">
+        <v>6</v>
+      </c>
+      <c r="C523">
+        <v>269</v>
+      </c>
+      <c r="D523">
+        <v>0</v>
+      </c>
+      <c r="E523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A524">
+        <v>24</v>
+      </c>
+      <c r="B524" t="s">
+        <v>5</v>
+      </c>
+      <c r="C524">
+        <v>269</v>
+      </c>
+      <c r="D524">
+        <v>0</v>
+      </c>
+      <c r="E524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A525">
+        <v>24</v>
+      </c>
+      <c r="B525" t="s">
+        <v>6</v>
+      </c>
+      <c r="C525">
+        <v>269</v>
+      </c>
+      <c r="D525">
+        <v>1</v>
+      </c>
+      <c r="E525">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A526">
+        <v>25</v>
+      </c>
+      <c r="B526" t="s">
+        <v>5</v>
+      </c>
+      <c r="C526">
+        <v>269</v>
+      </c>
+      <c r="D526">
+        <v>0</v>
+      </c>
+      <c r="E526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A527">
+        <v>25</v>
+      </c>
+      <c r="B527" t="s">
+        <v>6</v>
+      </c>
+      <c r="C527">
+        <v>269</v>
+      </c>
+      <c r="D527">
+        <v>1</v>
+      </c>
+      <c r="E527">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A528">
+        <v>26</v>
+      </c>
+      <c r="B528" t="s">
+        <v>5</v>
+      </c>
+      <c r="C528">
+        <v>269</v>
+      </c>
+      <c r="D528">
+        <v>5</v>
+      </c>
+      <c r="E528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A529">
+        <v>26</v>
+      </c>
+      <c r="B529" t="s">
+        <v>6</v>
+      </c>
+      <c r="C529">
+        <v>269</v>
+      </c>
+      <c r="D529">
+        <v>0</v>
+      </c>
+      <c r="E529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A530">
+        <v>27</v>
+      </c>
+      <c r="B530" t="s">
+        <v>5</v>
+      </c>
+      <c r="C530">
+        <v>269</v>
+      </c>
+      <c r="D530">
+        <v>0</v>
+      </c>
+      <c r="E530">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A531">
+        <v>27</v>
+      </c>
+      <c r="B531" t="s">
+        <v>6</v>
+      </c>
+      <c r="C531">
+        <v>269</v>
+      </c>
+      <c r="D531">
+        <v>1</v>
+      </c>
+      <c r="E531">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A532">
+        <v>28</v>
+      </c>
+      <c r="B532" t="s">
+        <v>5</v>
+      </c>
+      <c r="C532">
+        <v>269</v>
+      </c>
+      <c r="D532">
+        <v>0</v>
+      </c>
+      <c r="E532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A533">
+        <v>28</v>
+      </c>
+      <c r="B533" t="s">
+        <v>6</v>
+      </c>
+      <c r="C533">
+        <v>269</v>
+      </c>
+      <c r="D533">
+        <v>1</v>
+      </c>
+      <c r="E533">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A534">
+        <v>29</v>
+      </c>
+      <c r="B534" t="s">
+        <v>5</v>
+      </c>
+      <c r="C534">
+        <v>269</v>
+      </c>
+      <c r="D534">
+        <v>0</v>
+      </c>
+      <c r="E534">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A535">
+        <v>29</v>
+      </c>
+      <c r="B535" t="s">
+        <v>6</v>
+      </c>
+      <c r="C535">
+        <v>269</v>
+      </c>
+      <c r="D535">
+        <v>0</v>
+      </c>
+      <c r="E535">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A536">
+        <v>30</v>
+      </c>
+      <c r="B536" t="s">
+        <v>5</v>
+      </c>
+      <c r="C536">
+        <v>269</v>
+      </c>
+      <c r="D536">
+        <v>1</v>
+      </c>
+      <c r="E536">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A537">
+        <v>30</v>
+      </c>
+      <c r="B537" t="s">
+        <v>6</v>
+      </c>
+      <c r="C537">
+        <v>269</v>
+      </c>
+      <c r="D537">
+        <v>2</v>
+      </c>
+      <c r="E537">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A538">
+        <v>31</v>
+      </c>
+      <c r="B538" t="s">
+        <v>5</v>
+      </c>
+      <c r="C538">
+        <v>269</v>
+      </c>
+      <c r="D538">
+        <v>0</v>
+      </c>
+      <c r="E538">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A539">
+        <v>31</v>
+      </c>
+      <c r="B539" t="s">
+        <v>6</v>
+      </c>
+      <c r="C539">
+        <v>269</v>
+      </c>
+      <c r="D539">
+        <v>0</v>
+      </c>
+      <c r="E539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A540">
+        <v>32</v>
+      </c>
+      <c r="B540" t="s">
+        <v>5</v>
+      </c>
+      <c r="C540">
+        <v>269</v>
+      </c>
+      <c r="D540">
+        <v>1</v>
+      </c>
+      <c r="E540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A541">
+        <v>32</v>
+      </c>
+      <c r="B541" t="s">
+        <v>6</v>
+      </c>
+      <c r="C541">
+        <v>269</v>
+      </c>
+      <c r="D541">
+        <v>0</v>
+      </c>
+      <c r="E541">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A542">
+        <v>33</v>
+      </c>
+      <c r="B542" t="s">
+        <v>5</v>
+      </c>
+      <c r="C542">
+        <v>269</v>
+      </c>
+      <c r="D542">
+        <v>0</v>
+      </c>
+      <c r="E542">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A543">
+        <v>33</v>
+      </c>
+      <c r="B543" t="s">
+        <v>6</v>
+      </c>
+      <c r="C543">
+        <v>269</v>
+      </c>
+      <c r="D543">
+        <v>0</v>
+      </c>
+      <c r="E543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A544">
+        <v>34</v>
+      </c>
+      <c r="B544" t="s">
+        <v>5</v>
+      </c>
+      <c r="C544">
+        <v>269</v>
+      </c>
+      <c r="D544">
+        <v>1</v>
+      </c>
+      <c r="E544">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A545">
+        <v>34</v>
+      </c>
+      <c r="B545" t="s">
+        <v>6</v>
+      </c>
+      <c r="C545">
+        <v>269</v>
+      </c>
+      <c r="D545">
+        <v>1</v>
+      </c>
+      <c r="E545">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A546">
+        <v>1</v>
+      </c>
+      <c r="B546" t="s">
+        <v>5</v>
+      </c>
+      <c r="C546">
+        <v>282</v>
+      </c>
+      <c r="D546">
+        <v>0</v>
+      </c>
+      <c r="E546">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A547">
+        <v>1</v>
+      </c>
+      <c r="B547" t="s">
+        <v>6</v>
+      </c>
+      <c r="C547">
+        <v>282</v>
+      </c>
+      <c r="D547">
+        <v>0</v>
+      </c>
+      <c r="E547">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A548">
+        <v>2</v>
+      </c>
+      <c r="B548" t="s">
+        <v>5</v>
+      </c>
+      <c r="C548">
+        <v>282</v>
+      </c>
+      <c r="D548">
+        <v>1</v>
+      </c>
+      <c r="E548">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A549">
+        <v>2</v>
+      </c>
+      <c r="B549" t="s">
+        <v>6</v>
+      </c>
+      <c r="C549">
+        <v>282</v>
+      </c>
+      <c r="D549">
+        <v>0</v>
+      </c>
+      <c r="E549">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A550">
+        <v>3</v>
+      </c>
+      <c r="B550" t="s">
+        <v>5</v>
+      </c>
+      <c r="C550">
+        <v>282</v>
+      </c>
+      <c r="D550">
+        <v>2</v>
+      </c>
+      <c r="E550">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A551">
+        <v>3</v>
+      </c>
+      <c r="B551" t="s">
+        <v>6</v>
+      </c>
+      <c r="C551">
+        <v>282</v>
+      </c>
+      <c r="D551">
+        <v>0</v>
+      </c>
+      <c r="E551">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A552">
+        <v>4</v>
+      </c>
+      <c r="B552" t="s">
+        <v>5</v>
+      </c>
+      <c r="C552">
+        <v>282</v>
+      </c>
+      <c r="D552">
+        <v>0</v>
+      </c>
+      <c r="E552">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A553">
+        <v>4</v>
+      </c>
+      <c r="B553" t="s">
+        <v>6</v>
+      </c>
+      <c r="C553">
+        <v>282</v>
+      </c>
+      <c r="D553">
+        <v>0</v>
+      </c>
+      <c r="E553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A554">
+        <v>5</v>
+      </c>
+      <c r="B554" t="s">
+        <v>5</v>
+      </c>
+      <c r="C554">
+        <v>282</v>
+      </c>
+      <c r="D554">
+        <v>0</v>
+      </c>
+      <c r="E554">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A555">
+        <v>5</v>
+      </c>
+      <c r="B555" t="s">
+        <v>6</v>
+      </c>
+      <c r="C555">
+        <v>282</v>
+      </c>
+      <c r="D555">
+        <v>0</v>
+      </c>
+      <c r="E555">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A556">
+        <v>6</v>
+      </c>
+      <c r="B556" t="s">
+        <v>5</v>
+      </c>
+      <c r="C556">
+        <v>282</v>
+      </c>
+      <c r="D556">
+        <v>0</v>
+      </c>
+      <c r="E556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A557">
+        <v>6</v>
+      </c>
+      <c r="B557" t="s">
+        <v>6</v>
+      </c>
+      <c r="C557">
+        <v>282</v>
+      </c>
+      <c r="D557">
+        <v>0</v>
+      </c>
+      <c r="E557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A558">
+        <v>7</v>
+      </c>
+      <c r="B558" t="s">
+        <v>5</v>
+      </c>
+      <c r="C558">
+        <v>282</v>
+      </c>
+      <c r="D558">
+        <v>0</v>
+      </c>
+      <c r="E558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A559">
+        <v>7</v>
+      </c>
+      <c r="B559" t="s">
+        <v>6</v>
+      </c>
+      <c r="C559">
+        <v>282</v>
+      </c>
+      <c r="D559">
+        <v>0</v>
+      </c>
+      <c r="E559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A560">
+        <v>8</v>
+      </c>
+      <c r="B560" t="s">
+        <v>5</v>
+      </c>
+      <c r="C560">
+        <v>282</v>
+      </c>
+      <c r="D560">
+        <v>0</v>
+      </c>
+      <c r="E560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A561">
+        <v>8</v>
+      </c>
+      <c r="B561" t="s">
+        <v>6</v>
+      </c>
+      <c r="C561">
+        <v>282</v>
+      </c>
+      <c r="D561">
+        <v>3</v>
+      </c>
+      <c r="E561">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A562">
+        <v>9</v>
+      </c>
+      <c r="B562" t="s">
+        <v>5</v>
+      </c>
+      <c r="C562">
+        <v>282</v>
+      </c>
+      <c r="D562">
+        <v>0</v>
+      </c>
+      <c r="E562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A563">
+        <v>9</v>
+      </c>
+      <c r="B563" t="s">
+        <v>6</v>
+      </c>
+      <c r="C563">
+        <v>282</v>
+      </c>
+      <c r="D563">
+        <v>3</v>
+      </c>
+      <c r="E563">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A564">
+        <v>10</v>
+      </c>
+      <c r="B564" t="s">
+        <v>5</v>
+      </c>
+      <c r="C564">
+        <v>282</v>
+      </c>
+      <c r="D564">
+        <v>0</v>
+      </c>
+      <c r="E564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A565">
+        <v>10</v>
+      </c>
+      <c r="B565" t="s">
+        <v>6</v>
+      </c>
+      <c r="C565">
+        <v>282</v>
+      </c>
+      <c r="D565">
+        <v>0</v>
+      </c>
+      <c r="E565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A566">
+        <v>11</v>
+      </c>
+      <c r="B566" t="s">
+        <v>5</v>
+      </c>
+      <c r="C566">
+        <v>282</v>
+      </c>
+      <c r="D566">
+        <v>0</v>
+      </c>
+      <c r="E566">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A567">
+        <v>11</v>
+      </c>
+      <c r="B567" t="s">
+        <v>6</v>
+      </c>
+      <c r="C567">
+        <v>282</v>
+      </c>
+      <c r="D567">
+        <v>0</v>
+      </c>
+      <c r="E567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A568">
+        <v>12</v>
+      </c>
+      <c r="B568" t="s">
+        <v>5</v>
+      </c>
+      <c r="C568">
+        <v>282</v>
+      </c>
+      <c r="D568">
+        <v>0</v>
+      </c>
+      <c r="E568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A569">
+        <v>12</v>
+      </c>
+      <c r="B569" t="s">
+        <v>6</v>
+      </c>
+      <c r="C569">
+        <v>282</v>
+      </c>
+      <c r="D569">
+        <v>0</v>
+      </c>
+      <c r="E569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A570">
+        <v>13</v>
+      </c>
+      <c r="B570" t="s">
+        <v>5</v>
+      </c>
+      <c r="C570">
+        <v>282</v>
+      </c>
+      <c r="D570">
+        <v>0</v>
+      </c>
+      <c r="E570">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A571">
+        <v>13</v>
+      </c>
+      <c r="B571" t="s">
+        <v>6</v>
+      </c>
+      <c r="C571">
+        <v>282</v>
+      </c>
+      <c r="D571">
+        <v>0</v>
+      </c>
+      <c r="E571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A572">
+        <v>14</v>
+      </c>
+      <c r="B572" t="s">
+        <v>5</v>
+      </c>
+      <c r="C572">
+        <v>282</v>
+      </c>
+      <c r="D572">
+        <v>0</v>
+      </c>
+      <c r="E572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A573">
+        <v>14</v>
+      </c>
+      <c r="B573" t="s">
+        <v>6</v>
+      </c>
+      <c r="C573">
+        <v>282</v>
+      </c>
+      <c r="D573">
+        <v>0</v>
+      </c>
+      <c r="E573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A574">
+        <v>15</v>
+      </c>
+      <c r="B574" t="s">
+        <v>5</v>
+      </c>
+      <c r="C574">
+        <v>282</v>
+      </c>
+      <c r="D574">
+        <v>1</v>
+      </c>
+      <c r="E574">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A575">
+        <v>15</v>
+      </c>
+      <c r="B575" t="s">
+        <v>6</v>
+      </c>
+      <c r="C575">
+        <v>282</v>
+      </c>
+      <c r="D575">
+        <v>0</v>
+      </c>
+      <c r="E575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A576">
+        <v>16</v>
+      </c>
+      <c r="B576" t="s">
+        <v>5</v>
+      </c>
+      <c r="C576">
+        <v>282</v>
+      </c>
+      <c r="D576">
+        <v>1</v>
+      </c>
+      <c r="E576">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A577">
+        <v>16</v>
+      </c>
+      <c r="B577" t="s">
+        <v>6</v>
+      </c>
+      <c r="C577">
+        <v>282</v>
+      </c>
+      <c r="D577">
+        <v>2</v>
+      </c>
+      <c r="E577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A578">
+        <v>17</v>
+      </c>
+      <c r="B578" t="s">
+        <v>5</v>
+      </c>
+      <c r="C578">
+        <v>282</v>
+      </c>
+      <c r="D578">
+        <v>0</v>
+      </c>
+      <c r="E578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A579">
+        <v>17</v>
+      </c>
+      <c r="B579" t="s">
+        <v>6</v>
+      </c>
+      <c r="C579">
+        <v>282</v>
+      </c>
+      <c r="D579">
+        <v>0</v>
+      </c>
+      <c r="E579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A580">
+        <v>18</v>
+      </c>
+      <c r="B580" t="s">
+        <v>5</v>
+      </c>
+      <c r="C580">
+        <v>282</v>
+      </c>
+      <c r="D580">
+        <v>0</v>
+      </c>
+      <c r="E580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A581">
+        <v>18</v>
+      </c>
+      <c r="B581" t="s">
+        <v>6</v>
+      </c>
+      <c r="C581">
+        <v>282</v>
+      </c>
+      <c r="D581">
+        <v>0</v>
+      </c>
+      <c r="E581">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="582" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A582">
+        <v>19</v>
+      </c>
+      <c r="B582" t="s">
+        <v>5</v>
+      </c>
+      <c r="C582">
+        <v>282</v>
+      </c>
+      <c r="D582">
+        <v>0</v>
+      </c>
+      <c r="E582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A583">
+        <v>19</v>
+      </c>
+      <c r="B583" t="s">
+        <v>6</v>
+      </c>
+      <c r="C583">
+        <v>282</v>
+      </c>
+      <c r="D583">
+        <v>3</v>
+      </c>
+      <c r="E583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A584">
+        <v>20</v>
+      </c>
+      <c r="B584" t="s">
+        <v>5</v>
+      </c>
+      <c r="C584">
+        <v>282</v>
+      </c>
+      <c r="D584">
+        <v>1</v>
+      </c>
+      <c r="E584">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="585" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A585">
+        <v>20</v>
+      </c>
+      <c r="B585" t="s">
+        <v>6</v>
+      </c>
+      <c r="C585">
+        <v>282</v>
+      </c>
+      <c r="D585">
+        <v>0</v>
+      </c>
+      <c r="E585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A586">
+        <v>21</v>
+      </c>
+      <c r="B586" t="s">
+        <v>5</v>
+      </c>
+      <c r="C586">
+        <v>282</v>
+      </c>
+      <c r="D586">
+        <v>0</v>
+      </c>
+      <c r="E586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A587">
+        <v>21</v>
+      </c>
+      <c r="B587" t="s">
+        <v>6</v>
+      </c>
+      <c r="C587">
+        <v>282</v>
+      </c>
+      <c r="D587">
+        <v>2</v>
+      </c>
+      <c r="E587">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A588">
+        <v>22</v>
+      </c>
+      <c r="B588" t="s">
+        <v>5</v>
+      </c>
+      <c r="C588">
+        <v>282</v>
+      </c>
+      <c r="D588">
+        <v>0</v>
+      </c>
+      <c r="E588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A589">
+        <v>22</v>
+      </c>
+      <c r="B589" t="s">
+        <v>6</v>
+      </c>
+      <c r="C589">
+        <v>282</v>
+      </c>
+      <c r="D589">
+        <v>0</v>
+      </c>
+      <c r="E589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A590">
+        <v>23</v>
+      </c>
+      <c r="B590" t="s">
+        <v>5</v>
+      </c>
+      <c r="C590">
+        <v>282</v>
+      </c>
+      <c r="D590">
+        <v>0</v>
+      </c>
+      <c r="E590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A591">
+        <v>23</v>
+      </c>
+      <c r="B591" t="s">
+        <v>6</v>
+      </c>
+      <c r="C591">
+        <v>282</v>
+      </c>
+      <c r="D591">
+        <v>0</v>
+      </c>
+      <c r="E591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A592">
+        <v>24</v>
+      </c>
+      <c r="B592" t="s">
+        <v>5</v>
+      </c>
+      <c r="C592">
+        <v>282</v>
+      </c>
+      <c r="D592">
+        <v>0</v>
+      </c>
+      <c r="E592">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A593">
+        <v>24</v>
+      </c>
+      <c r="B593" t="s">
+        <v>6</v>
+      </c>
+      <c r="C593">
+        <v>282</v>
+      </c>
+      <c r="D593">
+        <v>1</v>
+      </c>
+      <c r="E593">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="594" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A594">
+        <v>25</v>
+      </c>
+      <c r="B594" t="s">
+        <v>5</v>
+      </c>
+      <c r="C594">
+        <v>282</v>
+      </c>
+      <c r="D594">
+        <v>0</v>
+      </c>
+      <c r="E594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A595">
+        <v>25</v>
+      </c>
+      <c r="B595" t="s">
+        <v>6</v>
+      </c>
+      <c r="C595">
+        <v>282</v>
+      </c>
+      <c r="D595">
+        <v>0</v>
+      </c>
+      <c r="E595">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A596">
+        <v>26</v>
+      </c>
+      <c r="B596" t="s">
+        <v>5</v>
+      </c>
+      <c r="C596">
+        <v>282</v>
+      </c>
+      <c r="D596">
+        <v>0</v>
+      </c>
+      <c r="E596">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A597">
+        <v>26</v>
+      </c>
+      <c r="B597" t="s">
+        <v>6</v>
+      </c>
+      <c r="C597">
+        <v>282</v>
+      </c>
+      <c r="D597">
+        <v>0</v>
+      </c>
+      <c r="E597">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A598">
+        <v>27</v>
+      </c>
+      <c r="B598" t="s">
+        <v>5</v>
+      </c>
+      <c r="C598">
+        <v>282</v>
+      </c>
+      <c r="D598">
+        <v>0</v>
+      </c>
+      <c r="E598">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A599">
+        <v>27</v>
+      </c>
+      <c r="B599" t="s">
+        <v>6</v>
+      </c>
+      <c r="C599">
+        <v>282</v>
+      </c>
+      <c r="D599">
+        <v>0</v>
+      </c>
+      <c r="E599">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A600">
+        <v>28</v>
+      </c>
+      <c r="B600" t="s">
+        <v>5</v>
+      </c>
+      <c r="C600">
+        <v>282</v>
+      </c>
+      <c r="D600">
+        <v>0</v>
+      </c>
+      <c r="E600">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A601">
+        <v>28</v>
+      </c>
+      <c r="B601" t="s">
+        <v>6</v>
+      </c>
+      <c r="C601">
+        <v>282</v>
+      </c>
+      <c r="D601">
+        <v>3</v>
+      </c>
+      <c r="E601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A602">
+        <v>29</v>
+      </c>
+      <c r="B602" t="s">
+        <v>5</v>
+      </c>
+      <c r="C602">
+        <v>282</v>
+      </c>
+      <c r="D602">
+        <v>0</v>
+      </c>
+      <c r="E602">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A603">
+        <v>29</v>
+      </c>
+      <c r="B603" t="s">
+        <v>6</v>
+      </c>
+      <c r="C603">
+        <v>282</v>
+      </c>
+      <c r="D603">
+        <v>0</v>
+      </c>
+      <c r="E603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A604">
+        <v>30</v>
+      </c>
+      <c r="B604" t="s">
+        <v>5</v>
+      </c>
+      <c r="C604">
+        <v>282</v>
+      </c>
+      <c r="D604">
+        <v>0</v>
+      </c>
+      <c r="E604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A605">
+        <v>30</v>
+      </c>
+      <c r="B605" t="s">
+        <v>6</v>
+      </c>
+      <c r="C605">
+        <v>282</v>
+      </c>
+      <c r="D605">
+        <v>0</v>
+      </c>
+      <c r="E605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A606">
+        <v>31</v>
+      </c>
+      <c r="B606" t="s">
+        <v>5</v>
+      </c>
+      <c r="C606">
+        <v>282</v>
+      </c>
+      <c r="D606">
+        <v>0</v>
+      </c>
+      <c r="E606">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A607">
+        <v>31</v>
+      </c>
+      <c r="B607" t="s">
+        <v>6</v>
+      </c>
+      <c r="C607">
+        <v>282</v>
+      </c>
+      <c r="D607">
+        <v>0</v>
+      </c>
+      <c r="E607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A608">
+        <v>32</v>
+      </c>
+      <c r="B608" t="s">
+        <v>5</v>
+      </c>
+      <c r="C608">
+        <v>282</v>
+      </c>
+      <c r="D608">
+        <v>3</v>
+      </c>
+      <c r="E608">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A609">
+        <v>32</v>
+      </c>
+      <c r="B609" t="s">
+        <v>6</v>
+      </c>
+      <c r="C609">
+        <v>282</v>
+      </c>
+      <c r="D609">
+        <v>2</v>
+      </c>
+      <c r="E609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A610">
+        <v>33</v>
+      </c>
+      <c r="B610" t="s">
+        <v>5</v>
+      </c>
+      <c r="C610">
+        <v>282</v>
+      </c>
+      <c r="D610">
+        <v>0</v>
+      </c>
+      <c r="E610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A611">
+        <v>33</v>
+      </c>
+      <c r="B611" t="s">
+        <v>6</v>
+      </c>
+      <c r="C611">
+        <v>282</v>
+      </c>
+      <c r="D611">
+        <v>0</v>
+      </c>
+      <c r="E611">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A612">
+        <v>34</v>
+      </c>
+      <c r="B612" t="s">
+        <v>5</v>
+      </c>
+      <c r="C612">
+        <v>282</v>
+      </c>
+      <c r="D612">
+        <v>0</v>
+      </c>
+      <c r="E612">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A613">
+        <v>34</v>
+      </c>
+      <c r="B613" t="s">
+        <v>6</v>
+      </c>
+      <c r="C613">
+        <v>282</v>
+      </c>
+      <c r="D613">
+        <v>0</v>
+      </c>
+      <c r="E613">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the data files with the new data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/fly_part2.xlsx
+++ b/data/fitness_development/fly_part2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_14/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFD7433-D11C-B24E-A6FD-F115AB11E9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{077DEEC6-D762-E444-AE5C-8E0DAE5890F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{BB242E00-5CB3-A84F-BA7A-96A75344F1EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BB242E00-5CB3-A84F-BA7A-96A75344F1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB267A-8CE1-0F4E-97AE-D44F1974EE08}">
-  <dimension ref="A1:E613"/>
+  <dimension ref="A1:E681"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A605" zoomScale="305" workbookViewId="0">
-      <selection activeCell="D614" sqref="D614"/>
+    <sheetView tabSelected="1" topLeftCell="A657" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F675" sqref="F675"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10860,6 +10860,1162 @@
         <v>0</v>
       </c>
     </row>
+    <row r="614" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A614">
+        <v>1</v>
+      </c>
+      <c r="B614" t="s">
+        <v>5</v>
+      </c>
+      <c r="C614">
+        <v>291</v>
+      </c>
+      <c r="D614">
+        <v>3</v>
+      </c>
+      <c r="E614">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A615">
+        <v>1</v>
+      </c>
+      <c r="B615" t="s">
+        <v>6</v>
+      </c>
+      <c r="C615">
+        <v>291</v>
+      </c>
+      <c r="D615">
+        <v>0</v>
+      </c>
+      <c r="E615">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A616">
+        <v>2</v>
+      </c>
+      <c r="B616" t="s">
+        <v>5</v>
+      </c>
+      <c r="C616">
+        <v>291</v>
+      </c>
+      <c r="D616">
+        <v>0</v>
+      </c>
+      <c r="E616">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="617" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A617">
+        <v>2</v>
+      </c>
+      <c r="B617" t="s">
+        <v>6</v>
+      </c>
+      <c r="C617">
+        <v>291</v>
+      </c>
+      <c r="D617">
+        <v>1</v>
+      </c>
+      <c r="E617">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="618" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A618">
+        <v>3</v>
+      </c>
+      <c r="B618" t="s">
+        <v>5</v>
+      </c>
+      <c r="C618">
+        <v>291</v>
+      </c>
+      <c r="D618">
+        <v>0</v>
+      </c>
+      <c r="E618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A619">
+        <v>3</v>
+      </c>
+      <c r="B619" t="s">
+        <v>6</v>
+      </c>
+      <c r="C619">
+        <v>291</v>
+      </c>
+      <c r="D619">
+        <v>2</v>
+      </c>
+      <c r="E619">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A620">
+        <v>4</v>
+      </c>
+      <c r="B620" t="s">
+        <v>5</v>
+      </c>
+      <c r="C620">
+        <v>291</v>
+      </c>
+      <c r="D620">
+        <v>5</v>
+      </c>
+      <c r="E620">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A621">
+        <v>4</v>
+      </c>
+      <c r="B621" t="s">
+        <v>6</v>
+      </c>
+      <c r="C621">
+        <v>291</v>
+      </c>
+      <c r="D621">
+        <v>0</v>
+      </c>
+      <c r="E621">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A622">
+        <v>5</v>
+      </c>
+      <c r="B622" t="s">
+        <v>5</v>
+      </c>
+      <c r="C622">
+        <v>291</v>
+      </c>
+      <c r="D622">
+        <v>1</v>
+      </c>
+      <c r="E622">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A623">
+        <v>5</v>
+      </c>
+      <c r="B623" t="s">
+        <v>6</v>
+      </c>
+      <c r="C623">
+        <v>291</v>
+      </c>
+      <c r="D623">
+        <v>1</v>
+      </c>
+      <c r="E623">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A624">
+        <v>6</v>
+      </c>
+      <c r="B624" t="s">
+        <v>5</v>
+      </c>
+      <c r="C624">
+        <v>291</v>
+      </c>
+      <c r="D624">
+        <v>0</v>
+      </c>
+      <c r="E624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A625">
+        <v>6</v>
+      </c>
+      <c r="B625" t="s">
+        <v>6</v>
+      </c>
+      <c r="C625">
+        <v>291</v>
+      </c>
+      <c r="D625">
+        <v>4</v>
+      </c>
+      <c r="E625">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A626">
+        <v>7</v>
+      </c>
+      <c r="B626" t="s">
+        <v>5</v>
+      </c>
+      <c r="C626">
+        <v>291</v>
+      </c>
+      <c r="D626">
+        <v>3</v>
+      </c>
+      <c r="E626">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A627">
+        <v>7</v>
+      </c>
+      <c r="B627" t="s">
+        <v>6</v>
+      </c>
+      <c r="C627">
+        <v>291</v>
+      </c>
+      <c r="D627">
+        <v>0</v>
+      </c>
+      <c r="E627">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A628">
+        <v>8</v>
+      </c>
+      <c r="B628" t="s">
+        <v>5</v>
+      </c>
+      <c r="C628">
+        <v>291</v>
+      </c>
+      <c r="D628">
+        <v>0</v>
+      </c>
+      <c r="E628">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A629">
+        <v>8</v>
+      </c>
+      <c r="B629" t="s">
+        <v>6</v>
+      </c>
+      <c r="C629">
+        <v>291</v>
+      </c>
+      <c r="D629">
+        <v>29</v>
+      </c>
+      <c r="E629">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="630" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A630">
+        <v>9</v>
+      </c>
+      <c r="B630" t="s">
+        <v>5</v>
+      </c>
+      <c r="C630">
+        <v>291</v>
+      </c>
+      <c r="D630">
+        <v>0</v>
+      </c>
+      <c r="E630">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A631">
+        <v>9</v>
+      </c>
+      <c r="B631" t="s">
+        <v>6</v>
+      </c>
+      <c r="C631">
+        <v>291</v>
+      </c>
+      <c r="D631">
+        <v>6</v>
+      </c>
+      <c r="E631">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A632">
+        <v>10</v>
+      </c>
+      <c r="B632" t="s">
+        <v>5</v>
+      </c>
+      <c r="C632">
+        <v>291</v>
+      </c>
+      <c r="D632">
+        <v>2</v>
+      </c>
+      <c r="E632">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A633">
+        <v>10</v>
+      </c>
+      <c r="B633" t="s">
+        <v>6</v>
+      </c>
+      <c r="C633">
+        <v>291</v>
+      </c>
+      <c r="D633">
+        <v>2</v>
+      </c>
+      <c r="E633">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A634">
+        <v>11</v>
+      </c>
+      <c r="B634" t="s">
+        <v>5</v>
+      </c>
+      <c r="C634">
+        <v>291</v>
+      </c>
+      <c r="D634">
+        <v>0</v>
+      </c>
+      <c r="E634">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A635">
+        <v>11</v>
+      </c>
+      <c r="B635" t="s">
+        <v>6</v>
+      </c>
+      <c r="C635">
+        <v>291</v>
+      </c>
+      <c r="D635">
+        <v>0</v>
+      </c>
+      <c r="E635">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A636">
+        <v>12</v>
+      </c>
+      <c r="B636" t="s">
+        <v>5</v>
+      </c>
+      <c r="C636">
+        <v>291</v>
+      </c>
+      <c r="D636">
+        <v>0</v>
+      </c>
+      <c r="E636">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A637">
+        <v>12</v>
+      </c>
+      <c r="B637" t="s">
+        <v>6</v>
+      </c>
+      <c r="C637">
+        <v>291</v>
+      </c>
+      <c r="D637">
+        <v>0</v>
+      </c>
+      <c r="E637">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="638" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A638">
+        <v>13</v>
+      </c>
+      <c r="B638" t="s">
+        <v>5</v>
+      </c>
+      <c r="C638">
+        <v>291</v>
+      </c>
+      <c r="D638">
+        <v>1</v>
+      </c>
+      <c r="E638">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="639" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A639">
+        <v>13</v>
+      </c>
+      <c r="B639" t="s">
+        <v>6</v>
+      </c>
+      <c r="C639">
+        <v>291</v>
+      </c>
+      <c r="D639">
+        <v>3</v>
+      </c>
+      <c r="E639">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A640">
+        <v>14</v>
+      </c>
+      <c r="B640" t="s">
+        <v>5</v>
+      </c>
+      <c r="C640">
+        <v>291</v>
+      </c>
+      <c r="D640">
+        <v>1</v>
+      </c>
+      <c r="E640">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="641" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A641">
+        <v>14</v>
+      </c>
+      <c r="B641" t="s">
+        <v>6</v>
+      </c>
+      <c r="C641">
+        <v>291</v>
+      </c>
+      <c r="D641">
+        <v>1</v>
+      </c>
+      <c r="E641">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="642" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A642">
+        <v>15</v>
+      </c>
+      <c r="B642" t="s">
+        <v>5</v>
+      </c>
+      <c r="C642">
+        <v>291</v>
+      </c>
+      <c r="D642">
+        <v>1</v>
+      </c>
+      <c r="E642">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="643" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A643">
+        <v>15</v>
+      </c>
+      <c r="B643" t="s">
+        <v>6</v>
+      </c>
+      <c r="C643">
+        <v>291</v>
+      </c>
+      <c r="D643">
+        <v>0</v>
+      </c>
+      <c r="E643">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A644">
+        <v>16</v>
+      </c>
+      <c r="B644" t="s">
+        <v>5</v>
+      </c>
+      <c r="C644">
+        <v>291</v>
+      </c>
+      <c r="D644">
+        <v>7</v>
+      </c>
+      <c r="E644">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="645" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A645">
+        <v>16</v>
+      </c>
+      <c r="B645" t="s">
+        <v>6</v>
+      </c>
+      <c r="C645">
+        <v>291</v>
+      </c>
+      <c r="D645">
+        <v>0</v>
+      </c>
+      <c r="E645">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A646">
+        <v>17</v>
+      </c>
+      <c r="B646" t="s">
+        <v>5</v>
+      </c>
+      <c r="C646">
+        <v>291</v>
+      </c>
+      <c r="D646">
+        <v>0</v>
+      </c>
+      <c r="E646">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="647" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A647">
+        <v>17</v>
+      </c>
+      <c r="B647" t="s">
+        <v>6</v>
+      </c>
+      <c r="C647">
+        <v>291</v>
+      </c>
+      <c r="D647">
+        <v>0</v>
+      </c>
+      <c r="E647">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A648">
+        <v>18</v>
+      </c>
+      <c r="B648" t="s">
+        <v>5</v>
+      </c>
+      <c r="C648">
+        <v>291</v>
+      </c>
+      <c r="D648">
+        <v>1</v>
+      </c>
+      <c r="E648">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A649">
+        <v>18</v>
+      </c>
+      <c r="B649" t="s">
+        <v>6</v>
+      </c>
+      <c r="C649">
+        <v>291</v>
+      </c>
+      <c r="D649">
+        <v>3</v>
+      </c>
+      <c r="E649">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="650" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A650">
+        <v>19</v>
+      </c>
+      <c r="B650" t="s">
+        <v>5</v>
+      </c>
+      <c r="C650">
+        <v>291</v>
+      </c>
+      <c r="D650">
+        <v>0</v>
+      </c>
+      <c r="E650">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A651">
+        <v>19</v>
+      </c>
+      <c r="B651" t="s">
+        <v>6</v>
+      </c>
+      <c r="C651">
+        <v>291</v>
+      </c>
+      <c r="D651">
+        <v>4</v>
+      </c>
+      <c r="E651">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A652">
+        <v>20</v>
+      </c>
+      <c r="B652" t="s">
+        <v>5</v>
+      </c>
+      <c r="C652">
+        <v>291</v>
+      </c>
+      <c r="D652">
+        <v>0</v>
+      </c>
+      <c r="E652">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A653">
+        <v>20</v>
+      </c>
+      <c r="B653" t="s">
+        <v>6</v>
+      </c>
+      <c r="C653">
+        <v>291</v>
+      </c>
+      <c r="D653">
+        <v>2</v>
+      </c>
+      <c r="E653">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="654" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A654">
+        <v>21</v>
+      </c>
+      <c r="B654" t="s">
+        <v>5</v>
+      </c>
+      <c r="C654">
+        <v>291</v>
+      </c>
+      <c r="D654">
+        <v>0</v>
+      </c>
+      <c r="E654">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="655" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A655">
+        <v>21</v>
+      </c>
+      <c r="B655" t="s">
+        <v>6</v>
+      </c>
+      <c r="C655">
+        <v>291</v>
+      </c>
+      <c r="D655">
+        <v>2</v>
+      </c>
+      <c r="E655">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="656" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A656">
+        <v>22</v>
+      </c>
+      <c r="B656" t="s">
+        <v>5</v>
+      </c>
+      <c r="C656">
+        <v>291</v>
+      </c>
+      <c r="D656">
+        <v>0</v>
+      </c>
+      <c r="E656">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="657" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A657">
+        <v>22</v>
+      </c>
+      <c r="B657" t="s">
+        <v>6</v>
+      </c>
+      <c r="C657">
+        <v>291</v>
+      </c>
+      <c r="D657">
+        <v>4</v>
+      </c>
+      <c r="E657">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A658">
+        <v>23</v>
+      </c>
+      <c r="B658" t="s">
+        <v>5</v>
+      </c>
+      <c r="C658">
+        <v>291</v>
+      </c>
+      <c r="D658">
+        <v>0</v>
+      </c>
+      <c r="E658">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A659">
+        <v>23</v>
+      </c>
+      <c r="B659" t="s">
+        <v>6</v>
+      </c>
+      <c r="C659">
+        <v>291</v>
+      </c>
+      <c r="D659">
+        <v>0</v>
+      </c>
+      <c r="E659">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A660">
+        <v>24</v>
+      </c>
+      <c r="B660" t="s">
+        <v>5</v>
+      </c>
+      <c r="C660">
+        <v>291</v>
+      </c>
+      <c r="D660">
+        <v>0</v>
+      </c>
+      <c r="E660">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A661">
+        <v>24</v>
+      </c>
+      <c r="B661" t="s">
+        <v>6</v>
+      </c>
+      <c r="C661">
+        <v>291</v>
+      </c>
+      <c r="D661">
+        <v>2</v>
+      </c>
+      <c r="E661">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="662" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A662">
+        <v>25</v>
+      </c>
+      <c r="B662" t="s">
+        <v>5</v>
+      </c>
+      <c r="C662">
+        <v>291</v>
+      </c>
+      <c r="D662">
+        <v>3</v>
+      </c>
+      <c r="E662">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A663">
+        <v>25</v>
+      </c>
+      <c r="B663" t="s">
+        <v>6</v>
+      </c>
+      <c r="C663">
+        <v>291</v>
+      </c>
+      <c r="D663">
+        <v>5</v>
+      </c>
+      <c r="E663">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="664" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A664">
+        <v>26</v>
+      </c>
+      <c r="B664" t="s">
+        <v>5</v>
+      </c>
+      <c r="C664">
+        <v>291</v>
+      </c>
+      <c r="D664">
+        <v>9</v>
+      </c>
+      <c r="E664">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A665">
+        <v>26</v>
+      </c>
+      <c r="B665" t="s">
+        <v>6</v>
+      </c>
+      <c r="C665">
+        <v>291</v>
+      </c>
+      <c r="D665">
+        <v>4</v>
+      </c>
+      <c r="E665">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A666">
+        <v>27</v>
+      </c>
+      <c r="B666" t="s">
+        <v>5</v>
+      </c>
+      <c r="C666">
+        <v>291</v>
+      </c>
+      <c r="D666">
+        <v>1</v>
+      </c>
+      <c r="E666">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="667" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A667">
+        <v>27</v>
+      </c>
+      <c r="B667" t="s">
+        <v>6</v>
+      </c>
+      <c r="C667">
+        <v>291</v>
+      </c>
+      <c r="D667">
+        <v>8</v>
+      </c>
+      <c r="E667">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="668" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A668">
+        <v>28</v>
+      </c>
+      <c r="B668" t="s">
+        <v>5</v>
+      </c>
+      <c r="C668">
+        <v>291</v>
+      </c>
+      <c r="D668">
+        <v>0</v>
+      </c>
+      <c r="E668">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="669" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A669">
+        <v>28</v>
+      </c>
+      <c r="B669" t="s">
+        <v>6</v>
+      </c>
+      <c r="C669">
+        <v>291</v>
+      </c>
+      <c r="D669">
+        <v>5</v>
+      </c>
+      <c r="E669">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="670" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A670">
+        <v>29</v>
+      </c>
+      <c r="B670" t="s">
+        <v>5</v>
+      </c>
+      <c r="C670">
+        <v>291</v>
+      </c>
+      <c r="D670">
+        <v>1</v>
+      </c>
+      <c r="E670">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="671" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A671">
+        <v>29</v>
+      </c>
+      <c r="B671" t="s">
+        <v>6</v>
+      </c>
+      <c r="C671">
+        <v>291</v>
+      </c>
+      <c r="D671">
+        <v>1</v>
+      </c>
+      <c r="E671">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="672" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A672">
+        <v>30</v>
+      </c>
+      <c r="B672" t="s">
+        <v>5</v>
+      </c>
+      <c r="C672">
+        <v>291</v>
+      </c>
+      <c r="D672">
+        <v>1</v>
+      </c>
+      <c r="E672">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="673" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A673">
+        <v>30</v>
+      </c>
+      <c r="B673" t="s">
+        <v>6</v>
+      </c>
+      <c r="C673">
+        <v>291</v>
+      </c>
+      <c r="D673">
+        <v>2</v>
+      </c>
+      <c r="E673">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A674">
+        <v>31</v>
+      </c>
+      <c r="B674" t="s">
+        <v>5</v>
+      </c>
+      <c r="C674">
+        <v>291</v>
+      </c>
+      <c r="D674">
+        <v>1</v>
+      </c>
+      <c r="E674">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="675" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A675">
+        <v>31</v>
+      </c>
+      <c r="B675" t="s">
+        <v>6</v>
+      </c>
+      <c r="C675">
+        <v>291</v>
+      </c>
+      <c r="D675">
+        <v>1</v>
+      </c>
+      <c r="E675">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="676" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A676">
+        <v>32</v>
+      </c>
+      <c r="B676" t="s">
+        <v>5</v>
+      </c>
+      <c r="C676">
+        <v>291</v>
+      </c>
+      <c r="D676">
+        <v>3</v>
+      </c>
+      <c r="E676">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A677">
+        <v>32</v>
+      </c>
+      <c r="B677" t="s">
+        <v>6</v>
+      </c>
+      <c r="C677">
+        <v>291</v>
+      </c>
+      <c r="D677">
+        <v>3</v>
+      </c>
+      <c r="E677">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A678">
+        <v>33</v>
+      </c>
+      <c r="B678" t="s">
+        <v>5</v>
+      </c>
+      <c r="C678">
+        <v>291</v>
+      </c>
+      <c r="D678">
+        <v>1</v>
+      </c>
+      <c r="E678">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="679" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A679">
+        <v>33</v>
+      </c>
+      <c r="B679" t="s">
+        <v>6</v>
+      </c>
+      <c r="C679">
+        <v>291</v>
+      </c>
+      <c r="D679">
+        <v>1</v>
+      </c>
+      <c r="E679">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="680" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A680">
+        <v>34</v>
+      </c>
+      <c r="B680" t="s">
+        <v>5</v>
+      </c>
+      <c r="C680">
+        <v>291</v>
+      </c>
+      <c r="D680">
+        <v>1</v>
+      </c>
+      <c r="E680">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="681" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A681">
+        <v>34</v>
+      </c>
+      <c r="B681" t="s">
+        <v>6</v>
+      </c>
+      <c r="C681">
+        <v>291</v>
+      </c>
+      <c r="D681">
+        <v>1</v>
+      </c>
+      <c r="E681">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>